<commit_message>
language v5.0 test results-1
</commit_message>
<xml_diff>
--- a/language.xlsx
+++ b/language.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="java" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,10 +15,13 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">go!$A$1:$I$1</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">java!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">python!$A$1:$I$29</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">python!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">java!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">python!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">java!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">python!$A$1:$I$29</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">python!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">go!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">go!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="102">
   <si>
     <t xml:space="preserve">测试项目</t>
   </si>
@@ -1868,7 +1871,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="M\／D\／YYYY"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1890,13 +1893,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Noto Sans CJK SC Regular"/>
-      <family val="2"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1965,6 +1961,7 @@
       <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -1979,6 +1976,7 @@
       <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -2007,6 +2005,7 @@
       <color rgb="FF000000"/>
       <name val="Noto Sans CJK SC Regular"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -2143,7 +2142,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2167,287 +2166,242 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="4" borderId="5" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="16" fillId="4" borderId="5" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="4" borderId="8" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="16" fillId="4" borderId="8" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="17" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="10" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="11" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="12" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="4" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="4" borderId="8" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="4" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal" xfId="21" builtinId="53" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF70AD47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF70AD47"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <b val="0"/>
@@ -2557,16 +2511,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.1481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.6148148148148"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="5.38888888888889"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="17.1481481481481"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="9.31111111111111"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.662962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.31111111111111"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="50.8592592592593"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="17.1481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="17.5407407407407"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="24.2037037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="5.48888888888889"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="17.5407407407407"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="9.5037037037037"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.7"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.9555555555556"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.5037037037037"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="52.1333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="17.5407407407407"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3114,7 +3068,7 @@
   </sheetPr>
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="I24" activeCellId="0" sqref="I24"/>
@@ -3122,16 +3076,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="11.8555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.6518518518518"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.91851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.91851851851852"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.5444444444444"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="27" width="8.91851851851852"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="38.5111111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.91851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="12.1518518518519"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.337037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.11481481481482"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.11481481481482"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="13.2296296296296"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.7407407407407"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="27" width="9.11481481481482"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="39.4925925925926"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.11481481481482"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3812,7 +3766,7 @@
       <c r="I29" s="37"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I29"/>
+  <autoFilter ref="A1:I1"/>
   <mergeCells count="2">
     <mergeCell ref="A2:A29"/>
     <mergeCell ref="D2:D29"/>
@@ -3856,24 +3810,24 @@
   </sheetPr>
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C36" activeCellId="0" sqref="C36"/>
+      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="11.8555555555556"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="31.6518518518518"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.91851851851852"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.91851851851852"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="12.937037037037"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.5444444444444"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="27" width="8.91851851851852"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="38.5111111111111"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.91851851851852"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="12.1518518518519"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.337037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.11481481481482"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.11481481481482"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="26" width="13.2296296296296"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.7407407407407"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="27" width="9.11481481481482"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="39.4925925925926"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.11481481481482"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="true" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3905,7 +3859,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" s="41" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="42" customFormat="true" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="38" t="s">
         <v>72</v>
       </c>
@@ -3924,11 +3878,15 @@
       <c r="F2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="40"/>
-    </row>
-    <row r="3" s="41" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="41"/>
+    </row>
+    <row r="3" s="42" customFormat="true" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="38"/>
       <c r="B3" s="39" t="s">
         <v>75</v>
@@ -3943,11 +3901,15 @@
       <c r="F3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="40"/>
-    </row>
-    <row r="4" s="41" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G3" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="41"/>
+    </row>
+    <row r="4" s="42" customFormat="true" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="38"/>
       <c r="B4" s="39" t="s">
         <v>76</v>
@@ -3962,11 +3924,15 @@
       <c r="F4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="13"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="40"/>
-    </row>
-    <row r="5" s="41" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G4" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="41"/>
+    </row>
+    <row r="5" s="42" customFormat="true" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="38"/>
       <c r="B5" s="39" t="s">
         <v>77</v>
@@ -3981,11 +3947,15 @@
       <c r="F5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="13"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="40"/>
-    </row>
-    <row r="6" s="41" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G5" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="41"/>
+    </row>
+    <row r="6" s="42" customFormat="true" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="38"/>
       <c r="B6" s="39" t="s">
         <v>78</v>
@@ -4000,11 +3970,15 @@
       <c r="F6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="13"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="40"/>
-    </row>
-    <row r="7" s="41" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G6" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="41"/>
+    </row>
+    <row r="7" s="42" customFormat="true" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="38"/>
       <c r="B7" s="39" t="s">
         <v>79</v>
@@ -4019,11 +3993,15 @@
       <c r="F7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="40"/>
-    </row>
-    <row r="8" s="41" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G7" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="41"/>
+    </row>
+    <row r="8" s="42" customFormat="true" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="38"/>
       <c r="B8" s="39" t="s">
         <v>80</v>
@@ -4038,11 +4016,15 @@
       <c r="F8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="40"/>
-    </row>
-    <row r="9" s="41" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G8" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="41"/>
+    </row>
+    <row r="9" s="42" customFormat="true" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="38"/>
       <c r="B9" s="39" t="s">
         <v>81</v>
@@ -4057,11 +4039,15 @@
       <c r="F9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="40"/>
-    </row>
-    <row r="10" s="41" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G9" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="41"/>
+    </row>
+    <row r="10" s="42" customFormat="true" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="38"/>
       <c r="B10" s="39" t="s">
         <v>82</v>
@@ -4076,11 +4062,15 @@
       <c r="F10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="40"/>
-    </row>
-    <row r="11" s="41" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G10" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="41"/>
+    </row>
+    <row r="11" s="42" customFormat="true" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="38"/>
       <c r="B11" s="39" t="s">
         <v>83</v>
@@ -4095,11 +4085,15 @@
       <c r="F11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="13"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="40"/>
-    </row>
-    <row r="12" s="41" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G11" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="41"/>
+    </row>
+    <row r="12" s="42" customFormat="true" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="38"/>
       <c r="B12" s="39" t="s">
         <v>84</v>
@@ -4114,11 +4108,15 @@
       <c r="F12" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="13"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="40"/>
-    </row>
-    <row r="13" s="41" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G12" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="41"/>
+    </row>
+    <row r="13" s="42" customFormat="true" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="38"/>
       <c r="B13" s="39" t="s">
         <v>85</v>
@@ -4133,11 +4131,15 @@
       <c r="F13" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="13"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="40"/>
-    </row>
-    <row r="14" s="41" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G13" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I13" s="41"/>
+    </row>
+    <row r="14" s="42" customFormat="true" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="38"/>
       <c r="B14" s="39" t="s">
         <v>86</v>
@@ -4152,11 +4154,15 @@
       <c r="F14" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="13"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="40"/>
-    </row>
-    <row r="15" s="41" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G14" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" s="41"/>
+    </row>
+    <row r="15" s="42" customFormat="true" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="38"/>
       <c r="B15" s="39" t="s">
         <v>87</v>
@@ -4171,11 +4177,15 @@
       <c r="F15" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="13"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="40"/>
-    </row>
-    <row r="16" s="41" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G15" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" s="41"/>
+    </row>
+    <row r="16" s="42" customFormat="true" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="38"/>
       <c r="B16" s="39" t="s">
         <v>88</v>
@@ -4190,222 +4200,270 @@
       <c r="F16" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="13"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="40"/>
+      <c r="G16" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I16" s="41"/>
     </row>
     <row r="17" s="49" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="42" t="s">
+      <c r="A17" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="45" t="s">
+      <c r="C17" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="E17" s="46" t="s">
+      <c r="E17" s="47" t="s">
         <v>43</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="13"/>
-      <c r="H17" s="47"/>
+      <c r="G17" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="40" t="s">
+        <v>43</v>
+      </c>
       <c r="I17" s="48"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="42"/>
+    <row r="18" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="43"/>
       <c r="B18" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="C18" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="45"/>
-      <c r="E18" s="46" t="s">
+      <c r="C18" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="46"/>
+      <c r="E18" s="47" t="s">
         <v>43</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="13"/>
-      <c r="H18" s="47"/>
+      <c r="G18" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="40" t="s">
+        <v>43</v>
+      </c>
       <c r="I18" s="48"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="42"/>
+    <row r="19" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="43"/>
       <c r="B19" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="45"/>
-      <c r="E19" s="46" t="s">
+      <c r="C19" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="46"/>
+      <c r="E19" s="47" t="s">
         <v>43</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G19" s="13"/>
-      <c r="H19" s="47"/>
+      <c r="G19" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H19" s="40" t="s">
+        <v>43</v>
+      </c>
       <c r="I19" s="48"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="42"/>
+    <row r="20" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="43"/>
       <c r="B20" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="C20" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="45"/>
-      <c r="E20" s="46" t="s">
+      <c r="C20" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="46"/>
+      <c r="E20" s="47" t="s">
         <v>43</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="13"/>
-      <c r="H20" s="47"/>
+      <c r="G20" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H20" s="40" t="s">
+        <v>43</v>
+      </c>
       <c r="I20" s="48"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="42"/>
+    <row r="21" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="43"/>
       <c r="B21" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="45"/>
-      <c r="E21" s="46" t="s">
+      <c r="C21" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="46"/>
+      <c r="E21" s="47" t="s">
         <v>43</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="13"/>
-      <c r="H21" s="47"/>
+      <c r="G21" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H21" s="40" t="s">
+        <v>43</v>
+      </c>
       <c r="I21" s="48"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="42"/>
+    <row r="22" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="43"/>
       <c r="B22" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="45"/>
-      <c r="E22" s="46" t="s">
+      <c r="C22" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="46"/>
+      <c r="E22" s="47" t="s">
         <v>43</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G22" s="13"/>
-      <c r="H22" s="47"/>
+      <c r="G22" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H22" s="40" t="s">
+        <v>43</v>
+      </c>
       <c r="I22" s="48"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="42"/>
+    <row r="23" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="43"/>
       <c r="B23" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="C23" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="45"/>
-      <c r="E23" s="46" t="s">
+      <c r="C23" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="46"/>
+      <c r="E23" s="47" t="s">
         <v>43</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="13"/>
-      <c r="H23" s="47"/>
+      <c r="G23" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H23" s="40" t="s">
+        <v>43</v>
+      </c>
       <c r="I23" s="48"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="42"/>
+    <row r="24" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="43"/>
       <c r="B24" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="C24" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="45"/>
-      <c r="E24" s="46" t="s">
+      <c r="C24" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="46"/>
+      <c r="E24" s="47" t="s">
         <v>43</v>
       </c>
       <c r="F24" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G24" s="13"/>
-      <c r="H24" s="47"/>
+      <c r="G24" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H24" s="40" t="s">
+        <v>43</v>
+      </c>
       <c r="I24" s="48"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="42"/>
+    <row r="25" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="43"/>
       <c r="B25" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="45"/>
-      <c r="E25" s="46" t="s">
+      <c r="C25" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="46"/>
+      <c r="E25" s="47" t="s">
         <v>43</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G25" s="13"/>
-      <c r="H25" s="47"/>
+      <c r="G25" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H25" s="40" t="s">
+        <v>43</v>
+      </c>
       <c r="I25" s="48"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="42"/>
+    <row r="26" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="43"/>
       <c r="B26" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="C26" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="45"/>
-      <c r="E26" s="46" t="s">
+      <c r="C26" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="46"/>
+      <c r="E26" s="47" t="s">
         <v>43</v>
       </c>
       <c r="F26" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G26" s="13"/>
-      <c r="H26" s="47"/>
+      <c r="G26" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H26" s="40" t="s">
+        <v>43</v>
+      </c>
       <c r="I26" s="48"/>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="42"/>
+    <row r="27" customFormat="false" ht="17.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="43"/>
       <c r="B27" s="50" t="s">
         <v>101</v>
       </c>
       <c r="C27" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="D27" s="45"/>
+      <c r="D27" s="46"/>
       <c r="E27" s="52" t="s">
         <v>43</v>
       </c>
       <c r="F27" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G27" s="23"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="54"/>
+      <c r="G27" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H27" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="I27" s="53"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1"/>
@@ -4423,11 +4481,7 @@
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H2:H16" type="list">
-      <formula1>"Pass通过,Fail失败,PLS Select请选择"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
+  <dataValidations count="2">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G2:G27" type="list">
       <formula1>"Pass,Fail"</formula1>
       <formula2>0</formula2>

</xml_diff>